<commit_message>
Change handling of dates to preserve original rows array for uploading
</commit_message>
<xml_diff>
--- a/ProgramExample.xlsx
+++ b/ProgramExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\ExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F60B2F-ED69-425A-8561-74529EC5F8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5C444-27E4-43CE-9AE0-6413393B16B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Room:</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>[v] Exhibition &amp; Eposter viewing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: </t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -230,6 +233,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,47 +504,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3">
+        <v>44807</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>0.3125</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -548,158 +547,158 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="403.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>0.3888888888888889</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>0.40277777777777773</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>0.4236111111111111</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>0.43055555555555558</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.4375</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>0.47916666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>0.5</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -708,12 +707,12 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>0.52083333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -722,12 +721,12 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -736,12 +735,12 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -750,12 +749,12 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -765,8 +764,12 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -846,6 +849,13 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove loading gif and replace with alert
</commit_message>
<xml_diff>
--- a/ProgramExample.xlsx
+++ b/ProgramExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\ExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5C444-27E4-43CE-9AE0-6413393B16B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E63A95-60F4-4BCB-A4C6-AA85E28082EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Remove unnecessary commented-out code
</commit_message>
<xml_diff>
--- a/ProgramExample.xlsx
+++ b/ProgramExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\ExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E63A95-60F4-4BCB-A4C6-AA85E28082EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC75A3D-7959-48D5-9CB6-4128BC71A65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Add ability to display multiple tables + minor styling changes + display speakers in table format
</commit_message>
<xml_diff>
--- a/ProgramExample.xlsx
+++ b/ProgramExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\ExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC75A3D-7959-48D5-9CB6-4128BC71A65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC85343-6766-4937-9525-4A42C52F035D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Room:</t>
   </si>
@@ -190,6 +190,21 @@
   </si>
   <si>
     <t xml:space="preserve">Date: </t>
+  </si>
+  <si>
+    <t>[n]</t>
+  </si>
+  <si>
+    <t>[s] Sample symposium</t>
+  </si>
+  <si>
+    <t>[e] Sample event</t>
+  </si>
+  <si>
+    <t>&lt;Sample speaker&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Speaker&gt;</t>
   </si>
 </sst>
 </file>
@@ -225,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -234,6 +249,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +629,9 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -778,38 +798,61 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3">
+        <v>44808</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4">
+        <v>44809</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -818,19 +861,39 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>

</xml_diff>